<commit_message>
tdf#104219 Don't export color information when color is automatic
In LibreOffice and MS Office, there are two types of colors:
 - Automatic (which is taken from settings) and Fixed (which is set by RGB value).
OOXML is setting automatic color by default, by not providing any RGB color.
To preserve automatic color we need to not export
RGB color during OOXML export.

Change-Id: I8895230c4fffc9d8741f3eff37e64c4823d71da8
Reviewed-on: https://gerrit.libreoffice.org/37970
Tested-by: Jenkins <ci@libreoffice.org>
Reviewed-by: Markus Mohrhard <markus.mohrhard@googlemail.com>
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/underlineColor.xlsx
+++ b/sc/qa/unit/data/xlsx/underlineColor.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,6 +58,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -66,16 +69,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>93345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -84,8 +87,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6296025" y="2409825"/>
-          <a:ext cx="1476375" cy="581025"/>
+          <a:off x="4238625" y="641985"/>
+          <a:ext cx="1476375" cy="558165"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -138,6 +141,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>211455</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>70485</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4221480" y="1524000"/>
+          <a:ext cx="1476375" cy="558165"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="25400" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="2800" b="1" u="heavy" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:uFillTx/>
+            </a:rPr>
+            <a:t>Text</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="2800" b="1" u="dbl" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:uFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="2800" b="1" u="dashLongHeavy" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:uFillTx/>
+            </a:rPr>
+            <a:t>Box</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -184,7 +283,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,7 +318,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -431,10 +530,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -447,7 +546,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -459,7 +558,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>